<commit_message>
new generaized datasheet reader added
</commit_message>
<xml_diff>
--- a/inst/reference_datasheet.xlsx
+++ b/inst/reference_datasheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19640"/>
   </bookViews>
   <sheets>
     <sheet name="dust_table_1.1" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="120">
   <si>
     <t>C Brn</t>
   </si>
   <si>
-    <t>C Blk</t>
-  </si>
-  <si>
     <t>C Gray</t>
   </si>
   <si>
@@ -306,9 +303,6 @@
     <t>Head</t>
   </si>
   <si>
-    <t xml:space="preserve">Human Hair Natural </t>
-  </si>
-  <si>
     <t xml:space="preserve">Human Hair Treated </t>
   </si>
   <si>
@@ -370,6 +364,21 @@
   </si>
   <si>
     <t>Section7</t>
+  </si>
+  <si>
+    <t>ColorNR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human Hair Natural      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C Blk  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">a note </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -885,7 +894,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="72">
+  <cellStyleXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -958,8 +967,12 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -970,8 +983,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="72">
+  <cellStyles count="76">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1015,6 +1029,8 @@
     <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1035,6 +1051,8 @@
     <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1348,13 +1366,14 @@
   <dimension ref="A1:R76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.1640625" customWidth="1"/>
     <col min="12" max="12" width="10.5" customWidth="1"/>
@@ -1366,43 +1385,43 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15" thickBot="1">
       <c r="A1" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="L1" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -1412,44 +1431,104 @@
     </row>
     <row r="2" spans="1:18" ht="15" thickTop="1">
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+      <c r="J2">
+        <v>8</v>
+      </c>
+      <c r="K2">
+        <v>9</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="B3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>13</v>
+      </c>
+      <c r="F3">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>15</v>
+      </c>
+      <c r="H3">
+        <v>16</v>
+      </c>
+      <c r="I3">
+        <v>17</v>
+      </c>
+      <c r="J3">
+        <v>18</v>
+      </c>
+      <c r="K3">
+        <v>19</v>
+      </c>
+      <c r="L3">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="B4" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15" thickBot="1">
       <c r="A5" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="K5" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -1461,58 +1540,82 @@
     </row>
     <row r="6" spans="1:18" ht="15" thickTop="1">
       <c r="B6" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="B7" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="B8" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15" thickBot="1">
       <c r="A9" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="L9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
@@ -1522,288 +1625,303 @@
     </row>
     <row r="10" spans="1:18" ht="15" thickTop="1">
       <c r="B10" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:18">
       <c r="B11" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="B12" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:18">
       <c r="B13" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:18">
       <c r="B14" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
+      </c>
+      <c r="I14" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:18">
       <c r="B15" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:18">
       <c r="B16" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:18">
       <c r="B17" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:18">
       <c r="B18" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:18">
       <c r="B19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="K19">
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:18">
       <c r="B20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:18">
       <c r="B21" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
+      </c>
+      <c r="H21" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:18">
       <c r="B22" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="15" thickBot="1">
       <c r="A23" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="G23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23" s="3" t="s">
+      <c r="H23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" s="3" t="s">
+      <c r="J23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="K23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="L23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="M23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M23" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="N23" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="O23" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="O23" s="3" t="s">
+      <c r="P23" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="P23" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="Q23" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R23" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="15" thickTop="1">
       <c r="B24" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:18">
       <c r="B25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:18">
       <c r="B26" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:18">
       <c r="B27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:18">
       <c r="B28" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:18">
       <c r="B29" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="15" thickBot="1">
       <c r="A30" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N30" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K30" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L30" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M30" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N30" s="3" t="s">
+      <c r="O30" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O30" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="P30" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q30" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R30" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="15" thickTop="1">
       <c r="B31" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:18">
       <c r="B32" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:18">
       <c r="B33" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:18">
       <c r="B34" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:18">
       <c r="B35" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:18">
       <c r="B36" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:18">
       <c r="B37" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:18">
       <c r="B38" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:18">
       <c r="B39" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:18">
       <c r="B40" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="15" thickBot="1">
       <c r="A41" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
@@ -1818,62 +1936,62 @@
     </row>
     <row r="42" spans="1:18" ht="15" thickTop="1">
       <c r="B42" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:18">
       <c r="B43" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:18">
       <c r="B44" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:18">
       <c r="B45" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:18">
       <c r="B46" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:18">
       <c r="B47" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:18">
       <c r="B48" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:18">
       <c r="B49" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:18">
       <c r="B50" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="1:18">
       <c r="B51" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:18">
       <c r="B52" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:18">
       <c r="B53" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
@@ -1894,15 +2012,17 @@
     </row>
     <row r="54" spans="1:18" ht="15" thickBot="1">
       <c r="A54" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D54" s="3"/>
+        <v>110</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
@@ -1920,112 +2040,112 @@
     </row>
     <row r="55" spans="1:18" ht="15" thickTop="1">
       <c r="B55" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:18">
       <c r="B56" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:18">
       <c r="B57" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:18">
       <c r="B58" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:18">
       <c r="B59" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:18">
       <c r="B60" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="61" spans="1:18">
       <c r="B61" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="62" spans="1:18">
       <c r="B62" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:18">
       <c r="B63" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="1:18">
       <c r="B64" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="67" spans="2:2">
       <c r="B67" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="2:2">
       <c r="B68" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="69" spans="2:2">
       <c r="B69" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="70" spans="2:2">
       <c r="B70" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="71" spans="2:2">
       <c r="B71" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="72" spans="2:2">
       <c r="B72" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="2:2">
       <c r="B73" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="74" spans="2:2">
       <c r="B74" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="75" spans="2:2">
       <c r="B75" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="76" spans="2:2">
       <c r="B76" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some cleanup in read data sheet routines
</commit_message>
<xml_diff>
--- a/inst/reference_datasheet.xlsx
+++ b/inst/reference_datasheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16340"/>
   </bookViews>
   <sheets>
     <sheet name="dust_table_1.1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="117">
   <si>
     <t>C Brn</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Yellow</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>Colorless</t>
   </si>
   <si>
@@ -258,9 +255,6 @@
     <t>Dyed Red</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Talc</t>
   </si>
   <si>
@@ -291,9 +285,6 @@
     <t>Starch Grains</t>
   </si>
   <si>
-    <t>Wood Fibers-Saw Dust</t>
-  </si>
-  <si>
     <t>ADD-Other</t>
   </si>
   <si>
@@ -375,10 +366,10 @@
     <t xml:space="preserve">C Blk  </t>
   </si>
   <si>
-    <t xml:space="preserve">a note </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  </t>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>Wood Fibers Saw Dust</t>
   </si>
 </sst>
 </file>
@@ -894,7 +885,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="76">
+  <cellStyleXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -971,6 +962,12 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -985,7 +982,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="76">
+  <cellStyles count="82">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1031,6 +1028,9 @@
     <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1053,6 +1053,9 @@
     <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1363,11 +1366,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R76"/>
+  <dimension ref="A1:R75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -1385,16 +1386,16 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15" thickBot="1">
       <c r="A1" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>1</v>
@@ -1418,10 +1419,10 @@
         <v>7</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -1431,85 +1432,28 @@
     </row>
     <row r="2" spans="1:18" ht="15" thickTop="1">
       <c r="B2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <v>6</v>
-      </c>
-      <c r="I2">
-        <v>7</v>
-      </c>
-      <c r="J2">
-        <v>8</v>
-      </c>
-      <c r="K2">
-        <v>9</v>
-      </c>
-      <c r="L2">
-        <v>10</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="B3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>12</v>
-      </c>
-      <c r="E3">
-        <v>13</v>
-      </c>
-      <c r="F3">
-        <v>14</v>
-      </c>
-      <c r="G3">
-        <v>15</v>
-      </c>
-      <c r="H3">
-        <v>16</v>
-      </c>
-      <c r="I3">
-        <v>17</v>
-      </c>
-      <c r="J3">
-        <v>18</v>
-      </c>
-      <c r="K3">
-        <v>19</v>
-      </c>
-      <c r="L3">
-        <v>20</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="B4" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
+      </c>
+      <c r="H4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15" thickBot="1">
       <c r="A5" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>8</v>
@@ -1528,7 +1472,7 @@
         <v>10</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -1540,46 +1484,22 @@
     </row>
     <row r="6" spans="1:18" ht="15" thickTop="1">
       <c r="B6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="B7" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="B8" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15" thickBot="1">
       <c r="A9" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>11</v>
@@ -1612,10 +1532,10 @@
         <v>20</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
@@ -1625,176 +1545,161 @@
     </row>
     <row r="10" spans="1:18" ht="15" thickTop="1">
       <c r="B10" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:18">
       <c r="B11" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="B12" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:18">
       <c r="B13" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:18">
       <c r="B14" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="I14" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:18">
       <c r="B15" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:18">
       <c r="B16" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:18">
       <c r="B17" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:18">
       <c r="B18" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:18">
       <c r="B19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K19">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:18">
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:18">
       <c r="B21" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H21" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:18">
       <c r="B22" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="15" thickBot="1">
       <c r="A23" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="K23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="L23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="M23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="M23" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="N23" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="O23" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="O23" s="3" t="s">
+      <c r="P23" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="P23" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="Q23" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R23" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="15" thickTop="1">
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:18">
       <c r="B25" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:18">
       <c r="B26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:18">
       <c r="B27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:18">
       <c r="B28" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:18">
       <c r="B29" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="15" thickBot="1">
       <c r="A30" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>12</v>
@@ -1824,95 +1729,92 @@
         <v>20</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N30" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O30" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="O30" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="P30" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q30" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R30" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="15" thickTop="1">
       <c r="B31" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:18">
       <c r="B32" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:18">
       <c r="B33" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F33" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:18">
       <c r="B34" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:18">
       <c r="B35" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:18">
       <c r="B36" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:18">
       <c r="B37" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:18">
       <c r="B38" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:18">
       <c r="B39" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:18">
       <c r="B40" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="15" thickBot="1">
       <c r="A41" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>16</v>
@@ -1921,7 +1823,7 @@
         <v>13</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
@@ -1936,62 +1838,62 @@
     </row>
     <row r="42" spans="1:18" ht="15" thickTop="1">
       <c r="B42" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:18">
       <c r="B43" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:18">
       <c r="B44" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:18">
       <c r="B45" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:18">
       <c r="B46" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:18">
       <c r="B47" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:18">
       <c r="B48" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:18">
       <c r="B49" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:18">
       <c r="B50" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:18">
       <c r="B51" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:18">
       <c r="B52" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:18">
       <c r="B53" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
@@ -2012,18 +1914,18 @@
     </row>
     <row r="54" spans="1:18" ht="15" thickBot="1">
       <c r="A54" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E54" s="3"/>
+        <v>88</v>
+      </c>
+      <c r="E54" s="7"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
@@ -2040,37 +1942,37 @@
     </row>
     <row r="55" spans="1:18" ht="15" thickTop="1">
       <c r="B55" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:18">
       <c r="B56" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:18">
       <c r="B57" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:18">
       <c r="B58" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:18">
       <c r="B59" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:18">
       <c r="B60" s="1" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
     </row>
     <row r="61" spans="1:18">
       <c r="B61" s="1" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:18">
@@ -2080,72 +1982,67 @@
     </row>
     <row r="63" spans="1:18">
       <c r="B63" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="64" spans="1:18">
       <c r="B64" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65" s="1" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66" s="1" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="2:2">
       <c r="B67" s="1" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="68" spans="2:2">
       <c r="B68" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="2:2">
       <c r="B69" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="70" spans="2:2">
       <c r="B70" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="71" spans="2:2">
       <c r="B71" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="72" spans="2:2">
       <c r="B72" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="73" spans="2:2">
       <c r="B73" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="74" spans="2:2">
       <c r="B74" s="1" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
     </row>
     <row r="75" spans="2:2">
-      <c r="B75" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="76" spans="2:2">
-      <c r="B76" s="6" t="s">
-        <v>91</v>
+      <c r="B75" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
constructing old2new datasheet converter
</commit_message>
<xml_diff>
--- a/inst/reference_datasheet.xlsx
+++ b/inst/reference_datasheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="dust_table_1.1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="117">
   <si>
     <t>C Brn</t>
   </si>
@@ -33,21 +33,12 @@
     <t>C Blonde</t>
   </si>
   <si>
-    <t xml:space="preserve">M </t>
-  </si>
-  <si>
-    <t xml:space="preserve">N </t>
-  </si>
-  <si>
     <t>MX Brn</t>
   </si>
   <si>
     <t>MX Other</t>
   </si>
   <si>
-    <t xml:space="preserve"> C </t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -219,9 +210,6 @@
     <t>Food Stuffs</t>
   </si>
   <si>
-    <t xml:space="preserve">Mineral Fibers </t>
-  </si>
-  <si>
     <t>Foam</t>
   </si>
   <si>
@@ -339,9 +327,6 @@
     <t>Slag/Mineral Wool</t>
   </si>
   <si>
-    <t>Glass/Mineral Grains</t>
-  </si>
-  <si>
     <t>Various</t>
   </si>
   <si>
@@ -363,13 +348,28 @@
     <t xml:space="preserve">Human Hair Natural      </t>
   </si>
   <si>
-    <t xml:space="preserve">C Blk  </t>
-  </si>
-  <si>
     <t xml:space="preserve">   </t>
   </si>
   <si>
     <t>Wood Fibers Saw Dust</t>
+  </si>
+  <si>
+    <t>C Blk</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Artifical Sweatners</t>
+  </si>
+  <si>
+    <t>Glitter</t>
+  </si>
+  <si>
+    <t>Minerals/Glass</t>
   </si>
 </sst>
 </file>
@@ -885,7 +885,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="82">
+  <cellStyleXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -968,6 +968,16 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -982,7 +992,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="82">
+  <cellStyles count="92">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1031,6 +1041,11 @@
     <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1056,6 +1071,11 @@
     <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1366,9 +1386,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R75"/>
+  <dimension ref="A1:T76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -1386,16 +1408,16 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15" thickBot="1">
       <c r="A1" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>1</v>
@@ -1407,22 +1429,22 @@
         <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="L1" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -1432,47 +1454,47 @@
     </row>
     <row r="2" spans="1:18" ht="15" thickTop="1">
       <c r="B2" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="B3" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="B4" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15" thickBot="1">
       <c r="A5" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
-        <v>4</v>
+        <v>112</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -1484,58 +1506,58 @@
     </row>
     <row r="6" spans="1:18" ht="15" thickTop="1">
       <c r="B6" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="B7" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="B8" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15" thickBot="1">
       <c r="A9" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="M9" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
@@ -1545,288 +1567,292 @@
     </row>
     <row r="10" spans="1:18" ht="15" thickTop="1">
       <c r="B10" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:18">
       <c r="B11" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="B12" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:18">
       <c r="B13" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:18">
       <c r="B14" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:18">
       <c r="B15" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:18">
       <c r="B16" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:18">
       <c r="B17" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:18">
       <c r="B18" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:18">
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:18">
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:18">
       <c r="B21" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:18">
       <c r="B22" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="15" thickBot="1">
       <c r="A23" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="H23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="3" t="s">
+      <c r="J23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="3" t="s">
+      <c r="K23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I23" s="3" t="s">
+      <c r="L23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="M23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K23" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="N23" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="R23" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="15" thickTop="1">
       <c r="B24" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:18">
       <c r="B25" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:18">
       <c r="B26" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:18">
       <c r="B27" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:18">
       <c r="B28" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:18">
       <c r="B29" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="15" thickBot="1">
       <c r="A30" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="H30" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="I30" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="J30" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="K30" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I30" s="3" t="s">
+      <c r="L30" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J30" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K30" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L30" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="M30" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="N30" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="Q30" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="R30" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="15" thickTop="1">
       <c r="B31" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:18">
       <c r="B32" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20">
+      <c r="B33" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20">
+      <c r="B34" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20">
+      <c r="B35" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
-      <c r="B33" s="1" t="s">
+    <row r="36" spans="1:20">
+      <c r="B36" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
-      <c r="B34" s="1" t="s">
+    <row r="37" spans="1:20">
+      <c r="B37" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
-      <c r="B35" s="1" t="s">
+    <row r="38" spans="1:20">
+      <c r="B38" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
-      <c r="B36" s="1" t="s">
+    <row r="39" spans="1:20">
+      <c r="B39" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
-      <c r="B37" s="1" t="s">
+    <row r="40" spans="1:20">
+      <c r="B40" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" ht="15" thickBot="1">
+      <c r="A41" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="38" spans="1:18">
-      <c r="B38" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18">
-      <c r="B39" s="1" t="s">
+      <c r="D41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="40" spans="1:18">
-      <c r="B40" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" ht="15" thickBot="1">
-      <c r="A41" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G41" s="3" t="s">
+      <c r="H41" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H41" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
+      <c r="I41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
@@ -1835,65 +1861,67 @@
       <c r="P41" s="3"/>
       <c r="Q41" s="3"/>
       <c r="R41" s="3"/>
-    </row>
-    <row r="42" spans="1:18" ht="15" thickTop="1">
+      <c r="S41" s="3"/>
+      <c r="T41" s="3"/>
+    </row>
+    <row r="42" spans="1:20" ht="15" thickTop="1">
       <c r="B42" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20">
+      <c r="B43" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20">
+      <c r="B44" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20">
+      <c r="B45" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20">
+      <c r="B46" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20">
+      <c r="B47" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:18">
-      <c r="B43" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18">
-      <c r="B44" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18">
-      <c r="B45" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18">
-      <c r="B46" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18">
-      <c r="B47" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:20">
       <c r="B48" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:18">
       <c r="B49" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:18">
       <c r="B50" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:18">
       <c r="B51" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:18">
       <c r="B52" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:18">
       <c r="B53" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
@@ -1914,16 +1942,16 @@
     </row>
     <row r="54" spans="1:18" ht="15" thickBot="1">
       <c r="A54" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B54" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C54" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C54" s="10" t="s">
-        <v>112</v>
-      </c>
       <c r="D54" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E54" s="7"/>
       <c r="F54" s="3"/>
@@ -1942,107 +1970,112 @@
     </row>
     <row r="55" spans="1:18" ht="15" thickTop="1">
       <c r="B55" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:18">
       <c r="B56" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:18">
       <c r="B57" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:18">
       <c r="B58" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:18">
       <c r="B59" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60" spans="1:18">
       <c r="B60" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" spans="1:18">
       <c r="B61" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:18">
       <c r="B62" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:18">
       <c r="B63" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64" spans="1:18">
       <c r="B64" s="1" t="s">
-        <v>65</v>
+        <v>114</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65" s="1" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66" s="1" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
     </row>
     <row r="67" spans="2:2">
       <c r="B67" s="1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="2:2">
       <c r="B68" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="69" spans="2:2">
       <c r="B69" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="70" spans="2:2">
       <c r="B70" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="2:2">
       <c r="B71" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="72" spans="2:2">
       <c r="B72" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="73" spans="2:2">
       <c r="B73" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="74" spans="2:2">
       <c r="B74" s="1" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
     </row>
     <row r="75" spans="2:2">
-      <c r="B75" s="6" t="s">
-        <v>88</v>
+      <c r="B75" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2">
+      <c r="B76" s="6" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on old datasheet conversions.
</commit_message>
<xml_diff>
--- a/inst/reference_datasheet.xlsx
+++ b/inst/reference_datasheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="5180" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="dust_table_1.1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="119">
   <si>
     <t>C Brn</t>
   </si>
@@ -369,7 +369,13 @@
     <t>Glitter</t>
   </si>
   <si>
-    <t>Minerals/Glass</t>
+    <t>Inorganic Fibers</t>
+  </si>
+  <si>
+    <t>Inorganic Grains</t>
+  </si>
+  <si>
+    <t>Section8</t>
   </si>
 </sst>
 </file>
@@ -885,7 +891,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="92">
+  <cellStyleXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -978,6 +984,24 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -992,7 +1016,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="92">
+  <cellStyles count="110">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1046,6 +1070,15 @@
     <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1076,6 +1109,15 @@
     <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1386,10 +1428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T76"/>
+  <dimension ref="A1:T77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1829,30 +1871,18 @@
       <c r="B41" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J41" s="7" t="s">
+      <c r="C41" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" s="7" t="s">
         <v>84</v>
       </c>
+      <c r="E41" s="7"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
@@ -1861,8 +1891,6 @@
       <c r="P41" s="3"/>
       <c r="Q41" s="3"/>
       <c r="R41" s="3"/>
-      <c r="S41" s="3"/>
-      <c r="T41" s="3"/>
     </row>
     <row r="42" spans="1:20" ht="15" thickTop="1">
       <c r="B42" s="1" t="s">
@@ -1879,12 +1907,49 @@
         <v>63</v>
       </c>
     </row>
-    <row r="45" spans="1:20">
-      <c r="B45" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20">
+    <row r="45" spans="1:20" ht="15" thickBot="1">
+      <c r="A45" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="O45" s="3"/>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3"/>
+      <c r="S45" s="8"/>
+      <c r="T45" s="8"/>
+    </row>
+    <row r="46" spans="1:20" ht="15" thickTop="1">
       <c r="B46" s="1" t="s">
         <v>50</v>
       </c>
@@ -1942,7 +2007,7 @@
     </row>
     <row r="54" spans="1:18" ht="15" thickBot="1">
       <c r="A54" s="4" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>102</v>
@@ -1975,106 +2040,111 @@
     </row>
     <row r="56" spans="1:18">
       <c r="B56" s="1" t="s">
-        <v>56</v>
+        <v>115</v>
       </c>
     </row>
     <row r="57" spans="1:18">
       <c r="B57" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:18">
       <c r="B58" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:18">
       <c r="B59" s="1" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:18">
       <c r="B60" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="1:18">
       <c r="B61" s="1" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="1:18">
       <c r="B62" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:18">
       <c r="B63" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:18">
       <c r="B64" s="1" t="s">
-        <v>114</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65" s="1" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66" s="1" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="2:2">
       <c r="B67" s="1" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
     </row>
     <row r="68" spans="2:2">
       <c r="B68" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="69" spans="2:2">
       <c r="B69" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="70" spans="2:2">
       <c r="B70" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="71" spans="2:2">
       <c r="B71" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="72" spans="2:2">
       <c r="B72" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="73" spans="2:2">
       <c r="B73" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="74" spans="2:2">
       <c r="B74" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="75" spans="2:2">
       <c r="B75" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2">
+      <c r="B76" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="76" spans="2:2">
-      <c r="B76" s="6" t="s">
+    <row r="77" spans="2:2">
+      <c r="B77" s="6" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>